<commit_message>
fix some text file issues
</commit_message>
<xml_diff>
--- a/stimuli/Text_stimuli.xlsx
+++ b/stimuli/Text_stimuli.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\SPR_online\stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78D7B8C-6696-4BEC-A6E3-01BD44C5B13E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6066119-F445-46C7-A8D6-0CB25335ADA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14460" yWindow="3630" windowWidth="20475" windowHeight="17070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -57,36 +57,18 @@
     <t>Q2_ans</t>
   </si>
   <si>
-    <t>I agree that California's "three strikes and you're out" law will be a financial disaster for
-taxpayers who care about education and other vital services. But it's far from clear that the law
-can even be credited with a reduction in crime in California. While it's true that crime declined
-in California last year, crime also dropped nationwide.</t>
-  </si>
-  <si>
     <t>Last year, crime declined in California, but not nationwide.</t>
   </si>
   <si>
     <t>Richard Carrington was observing the sun.</t>
   </si>
   <si>
-    <t>Dorothy didn't know. She looked around her anxiously for some familiar landmark; but everything was
-strange. Between the branches of the many roads were green meadows and a few shrubs and trees, but
-she couldn't see the farm-house from which she had just come, or anything she had ever seen before,
-except the shaggy man and Toto.</t>
-  </si>
-  <si>
     <t>Dorothy couldn't recognise nearby landmarks.</t>
   </si>
   <si>
     <t>His did not keep notes of his observations</t>
   </si>
   <si>
-    <t>Known as Rapa Nui to the island's inhabitants, Rongorongo is a writing system comprised of
-pictographs. It has been found carved into many oblong wooden tablets and other artifacts from the
-island's history. The art of writing was not known in any nearby islands and the script's mere
-existence is sufficient to confound anthropologists.</t>
-  </si>
-  <si>
     <t>The writing script was found on other islands in the area.</t>
   </si>
   <si>
@@ -181,6 +163,15 @@
   </si>
   <si>
     <t>The United States and Colombia have the same rule for declaring cash.</t>
+  </si>
+  <si>
+    <t>I agree that California's "three strikes and you're out" law will be a financial disaster for taxpayers who care about education and other vital services. But it's far from clear that the law can even be credited with a reduction in crime in California. While it's true that crime declined in California last year, crime also dropped nationwide.</t>
+  </si>
+  <si>
+    <t>Dorothy didn't know. She looked around her anxiously for some familiar landmark; but everything was strange. Between the branches of the many roads were green meadows and a few shrubs and trees, but she couldn't see the farm-house from which she had just come, or anything she had ever seen before, except the shaggy man and Toto.</t>
+  </si>
+  <si>
+    <t>Known as Rapa Nui to the island's inhabitants, Rongorongo is a writing system comprised of pictographs. It has been found carved into many oblong wooden tablets and other artifacts from the island's history. The art of writing was not known in any nearby islands and the script's mere existence is sufficient to confound anthropologists.</t>
   </si>
 </sst>
 </file>
@@ -532,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +562,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -582,16 +573,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2">
         <v>0</v>
@@ -601,7 +592,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -609,26 +600,26 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="G3" s="2">
         <v>0</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -636,26 +627,26 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -663,23 +654,23 @@
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G5" s="2">
         <v>1</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -690,16 +681,16 @@
         <v>12</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G6" s="2">
         <v>1</v>
@@ -717,16 +708,16 @@
         <v>14</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G7" s="2">
         <v>1</v>
@@ -744,16 +735,16 @@
         <v>15</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G8" s="2">
         <v>1</v>
@@ -771,16 +762,16 @@
         <v>18</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G9" s="2">
         <v>1</v>
@@ -798,16 +789,16 @@
         <v>40</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G10" s="2">
         <v>0</v>
@@ -825,7 +816,7 @@
         <v>43</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="0"/>
@@ -840,10 +831,10 @@
         <v>48</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
@@ -861,16 +852,16 @@
         <v>52</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E13" s="2">
         <v>0</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G13" s="2">
         <v>0</v>
@@ -888,7 +879,7 @@
         <v>53</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="0"/>
@@ -903,7 +894,7 @@
         <v>54</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="0"/>
@@ -918,16 +909,16 @@
         <v>55</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E16" s="2">
         <v>0</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G16" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
update with more lab.js programming
</commit_message>
<xml_diff>
--- a/stimuli/Text_stimuli.xlsx
+++ b/stimuli/Text_stimuli.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\SPR_online\stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E124A5D0-267E-461D-8B62-FB43B21E7B73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7826E80-258A-4397-BC6D-D4D5D9AD58A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>Dorothy couldn't recognise the nearby landmarks.</t>
+  </si>
+  <si>
+    <t>According to common wisdom, feeling close to your partner is not important.</t>
+  </si>
+  <si>
+    <t>According to the new study, the degree to which a person wants to be close to their partner is what matters the most.</t>
   </si>
 </sst>
 </file>
@@ -527,7 +533,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +597,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="2">
-        <f>IF(ISBLANK(C2),0,LEN(TRIM(C2))-LEN(SUBSTITUTE(C2," ",""))+1)</f>
+        <f t="shared" ref="H2:H16" si="0">IF(ISBLANK(C2),0,LEN(TRIM(C2))-LEN(SUBSTITUTE(C2," ",""))+1)</f>
         <v>59</v>
       </c>
     </row>
@@ -618,7 +624,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="2">
-        <f>IF(ISBLANK(C3),0,LEN(TRIM(C3))-LEN(SUBSTITUTE(C3," ",""))+1)</f>
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
     </row>
@@ -645,7 +651,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="2">
-        <f>IF(ISBLANK(C4),0,LEN(TRIM(C4))-LEN(SUBSTITUTE(C4," ",""))+1)</f>
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
     </row>
@@ -672,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="2">
-        <f>IF(ISBLANK(C5),0,LEN(TRIM(C5))-LEN(SUBSTITUTE(C5," ",""))+1)</f>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
     </row>
@@ -699,7 +705,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="2">
-        <f>IF(ISBLANK(C6),0,LEN(TRIM(C6))-LEN(SUBSTITUTE(C6," ",""))+1)</f>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
     </row>
@@ -726,7 +732,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="2">
-        <f>IF(ISBLANK(C7),0,LEN(TRIM(C7))-LEN(SUBSTITUTE(C7," ",""))+1)</f>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
     </row>
@@ -753,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="2">
-        <f>IF(ISBLANK(C8),0,LEN(TRIM(C8))-LEN(SUBSTITUTE(C8," ",""))+1)</f>
+        <f t="shared" si="0"/>
         <v>53</v>
       </c>
     </row>
@@ -780,7 +786,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="2">
-        <f>IF(ISBLANK(C9),0,LEN(TRIM(C9))-LEN(SUBSTITUTE(C9," ",""))+1)</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
     </row>
@@ -807,7 +813,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="2">
-        <f>IF(ISBLANK(C10),0,LEN(TRIM(C10))-LEN(SUBSTITUTE(C10," ",""))+1)</f>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
     </row>
@@ -834,7 +840,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="2">
-        <f>IF(ISBLANK(C11),0,LEN(TRIM(C11))-LEN(SUBSTITUTE(C11," ",""))+1)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
@@ -861,7 +867,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="2">
-        <f>IF(ISBLANK(C12),0,LEN(TRIM(C12))-LEN(SUBSTITUTE(C12," ",""))+1)</f>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
     </row>
@@ -888,7 +894,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="2">
-        <f>IF(ISBLANK(C13),0,LEN(TRIM(C13))-LEN(SUBSTITUTE(C13," ",""))+1)</f>
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
     </row>
@@ -903,7 +909,7 @@
         <v>24</v>
       </c>
       <c r="H14" s="2">
-        <f>IF(ISBLANK(C14),0,LEN(TRIM(C14))-LEN(SUBSTITUTE(C14," ",""))+1)</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
     </row>
@@ -917,8 +923,20 @@
       <c r="C15" s="6" t="s">
         <v>25</v>
       </c>
+      <c r="D15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
       <c r="H15" s="2">
-        <f>IF(ISBLANK(C15),0,LEN(TRIM(C15))-LEN(SUBSTITUTE(C15," ",""))+1)</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
     </row>
@@ -933,7 +951,7 @@
         <v>19</v>
       </c>
       <c r="H16" s="2">
-        <f>IF(ISBLANK(C16),0,LEN(TRIM(C16))-LEN(SUBSTITUTE(C16," ",""))+1)</f>
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update after changes to experiment
</commit_message>
<xml_diff>
--- a/stimuli/Text_stimuli.xlsx
+++ b/stimuli/Text_stimuli.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\SPR_online\stimuli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3E37C2-B61B-4FA9-9C1D-251AD81A3C9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B706D46-92CB-48C3-A9A7-09550A39D64A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Richard Carrington was observing sunspots.</t>
   </si>
   <si>
-    <t>Police shut down the lemonade stand, saying the girls weren't old enough to run it.</t>
-  </si>
-  <si>
     <t>The snowstorm happened during the weekend.</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
     <t>Michael Larson wanted to empty his whole bank account.</t>
   </si>
   <si>
-    <t>His did not keep notes of his observations</t>
-  </si>
-  <si>
     <t>Dorothy couldn't recognise any nearby landmarks.</t>
   </si>
   <si>
@@ -184,6 +178,39 @@
   </si>
   <si>
     <t>The girls ran the lemonade stand to save money for a new toy.</t>
+  </si>
+  <si>
+    <t>Richard Carrington did not keep notes of his observations.</t>
+  </si>
+  <si>
+    <t>Police shut down the lemonade stand because the girls weren't old enough to run it.</t>
+  </si>
+  <si>
+    <t>American industry may not know it, but debate in Congress over reforming the federal government's regulatory apparatus may profoundly improve companies' ability to survive. This week the Senate seems poised to join the House in a massive overhaul of the way in which bureaucrats enact regulations that are strangling the life out of companies.</t>
+  </si>
+  <si>
+    <t>According to the passage, the Senate and the House are expected to work together on the reforms.</t>
+  </si>
+  <si>
+    <t>Owls are more flexible than humans because a bird's head is only connected by one socket pivot. People have two, which limits our ability to twist, Forsman added. Owls also have multiple vertebrae, the small bones that make up the neck and spine, helping them achieve a wide range of motion.</t>
+  </si>
+  <si>
+    <t>A bill was drafted and introduced into Parliament several times but met with great opposition, mostly from farmers. Eventually, in 1925, it was decided that summer time should begin on the day following the third Saturday in April and close after the first Saturday in October.</t>
+  </si>
+  <si>
+    <t>The bill was mostly opposed by bankers.</t>
+  </si>
+  <si>
+    <t>According to the passage, humans are more flexible than owls.</t>
+  </si>
+  <si>
+    <t>According to the passage, the debate in Congress is not likely to affect the survival of American companies.</t>
+  </si>
+  <si>
+    <t>According to the passage, the ability to twist depends on our muscle strength.</t>
+  </si>
+  <si>
+    <t>The bill was introduced into Parliament more than once.</t>
   </si>
 </sst>
 </file>
@@ -207,7 +234,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,6 +244,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -233,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -255,6 +288,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,13 +642,13 @@
         <v>1</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G2" s="7">
         <v>0</v>
       </c>
       <c r="H2" s="2">
-        <f t="shared" ref="H2:H15" si="0">IF(ISBLANK(C2),0,LEN(TRIM(C2))-LEN(SUBSTITUTE(C2," ",""))+1)</f>
+        <f t="shared" ref="H2:H18" si="0">IF(ISBLANK(C2),0,LEN(TRIM(C2))-LEN(SUBSTITUTE(C2," ",""))+1)</f>
         <v>59</v>
       </c>
     </row>
@@ -645,7 +690,7 @@
         <v>31</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E4" s="7">
         <v>1</v>
@@ -678,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G5" s="7">
         <v>1</v>
@@ -699,7 +744,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="7">
         <v>1</v>
@@ -726,13 +771,13 @@
         <v>12</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="7">
         <v>1</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G7" s="7">
         <v>0</v>
@@ -780,7 +825,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="7">
         <v>0</v>
@@ -808,13 +853,13 @@
         <v>15</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="E10" s="7">
-        <v>0</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="G10" s="7">
         <v>0</v>
@@ -906,89 +951,174 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="9">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9">
+        <v>51</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="9">
+        <v>1</v>
+      </c>
+      <c r="H14" s="9">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9">
+        <v>17</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0</v>
+      </c>
+      <c r="H15" s="9">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>15</v>
+      </c>
+      <c r="B16" s="9">
+        <v>28</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="9">
+        <v>1</v>
+      </c>
+      <c r="H16" s="9">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>99</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B17" s="2">
         <v>53</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2" t="s">
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="2">
-        <v>1</v>
-      </c>
-      <c r="H14" s="2">
+      <c r="G17" s="2">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>100</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B18" s="2">
         <v>54</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2">
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="4"/>
-      <c r="H18" s="2">
-        <f>SUM(H2:H13)</f>
-        <v>650</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C19" s="4"/>
-      <c r="H19" s="2">
-        <f>SUM(H3:H13)/3 -12</f>
-        <v>185</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C20" s="4"/>
-      <c r="E20" s="2">
-        <f>SUM(E2:E13, G2:G13)/(12*2)</f>
-        <v>0.45833333333333331</v>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="4"/>
+      <c r="H21" s="2">
+        <f>SUM(H2:H16)</f>
+        <v>801</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="4"/>
+      <c r="H22" s="2">
+        <f>SUM(H3:H16)/3 -15</f>
+        <v>232.33333333333334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="4"/>
+      <c r="E23" s="2">
+        <f>SUM(E2:E16, G2:G16)/(15*2)</f>
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="H23" s="2">
+        <f>AVERAGE(H2:H16)-1</f>
+        <v>52.4</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q20">
-    <sortCondition ref="A2:A20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q23">
+    <sortCondition ref="A2:A23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>